<commit_message>
add DR category codes and DR.class element to profiles and min valueset extension to DR.type
</commit_message>
<xml_diff>
--- a/docs/cn-plus-uscore.xlsx
+++ b/docs/cn-plus-uscore.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="415">
   <si>
     <t>Path</t>
   </si>
@@ -462,10 +462,10 @@
     <t>Specifies the particular kind of document referenced  (e.g. History and Physical, Discharge Summary, Progress Note). This usually equates to the purpose of making the document referenced.</t>
   </si>
   <si>
-    <t>Key metadata element describing the document, used in searching/filtering.</t>
-  </si>
-  <si>
-    <t>Provider role codes consisting of NUCC Health Care Provider Taxonomy Code Set for providers.</t>
+    <t>The `DocumentReference.type` binding must support at a minimum these [6 concepts](ValueSet-dr-type.html) and may extend to the full  [HITSP C80 Table 2-144 Document Class Value Set Definition](http://build.fhir.org/valueset-c80-doc-typecodes.html)</t>
+  </si>
+  <si>
+    <t>This is the code specifying the precise type of document</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/c80-doc-typecodes</t>
@@ -502,13 +502,7 @@
     <t>Helps humans to assess whether the document is of interest when viewing a list of documents.</t>
   </si>
   <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>High-level kind of a clinical document at a macro level.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/c80-doc-classcodes</t>
+    <t>http://fhir.org/guides/argonaut-clinicalnotes/ValueSet/dr-category</t>
   </si>
   <si>
     <t>.outboundRelationship[typeCode="COMP].target[classCode="LIST", moodCode="EVN"].code</t>
@@ -1147,6 +1141,9 @@
   </si>
   <si>
     <t>An event can further specialize the act inherent in the type, such as  where it is simply "Procedure Report" and the procedure was a "colonoscopy". If one or more event codes are included, they shall not conflict with the values inherent in the class or type elements as such a conflict would create an ambiguous situation.</t>
+  </si>
+  <si>
+    <t>example</t>
   </si>
   <si>
     <t>This list of codes represents the main clinical acts being documented.</t>
@@ -1480,8 +1477,8 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="91.1328125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="55.90625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="75.515625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="66.0234375" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="43.0625" customWidth="true" bestFit="true"/>
@@ -3167,7 +3164,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>150</v>
       </c>
@@ -3177,13 +3174,13 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s" s="2">
         <v>50</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>40</v>
@@ -3229,13 +3226,11 @@
         <v>40</v>
       </c>
       <c r="W16" t="s" s="2">
+        <v>73</v>
+      </c>
+      <c r="X16" s="2"/>
+      <c r="Y16" t="s" s="2">
         <v>156</v>
-      </c>
-      <c r="X16" t="s" s="2">
-        <v>157</v>
-      </c>
-      <c r="Y16" t="s" s="2">
-        <v>158</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>40</v>
@@ -3268,7 +3263,7 @@
         <v>40</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>147</v>
@@ -3277,12 +3272,12 @@
         <v>40</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -3305,13 +3300,13 @@
         <v>51</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>160</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>161</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>162</v>
-      </c>
-      <c r="K17" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="L17" t="s" s="2">
-        <v>164</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -3362,7 +3357,7 @@
         <v>40</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>41</v>
@@ -3377,21 +3372,21 @@
         <v>40</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="AK17" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="AL17" t="s" s="2">
         <v>165</v>
       </c>
-      <c r="AK17" t="s" s="2">
+      <c r="AM17" t="s" s="2">
         <v>166</v>
-      </c>
-      <c r="AL17" t="s" s="2">
-        <v>167</v>
-      </c>
-      <c r="AM17" t="s" s="2">
-        <v>168</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3414,16 +3409,16 @@
         <v>51</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>168</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>169</v>
+      </c>
+      <c r="L18" t="s" s="2">
         <v>170</v>
       </c>
-      <c r="K18" t="s" s="2">
+      <c r="M18" t="s" s="2">
         <v>171</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>173</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
@@ -3473,7 +3468,7 @@
         <v>40</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>41</v>
@@ -3488,21 +3483,21 @@
         <v>40</v>
       </c>
       <c r="AJ18" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="AK18" t="s" s="2">
+        <v>173</v>
+      </c>
+      <c r="AL18" t="s" s="2">
         <v>174</v>
       </c>
-      <c r="AK18" t="s" s="2">
+      <c r="AM18" t="s" s="2">
         <v>175</v>
-      </c>
-      <c r="AL18" t="s" s="2">
-        <v>176</v>
-      </c>
-      <c r="AM18" t="s" s="2">
-        <v>177</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3525,16 +3520,16 @@
         <v>51</v>
       </c>
       <c r="J19" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="K19" t="s" s="2">
+        <v>178</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>179</v>
       </c>
-      <c r="K19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>180</v>
-      </c>
-      <c r="L19" t="s" s="2">
-        <v>181</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>182</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3584,7 +3579,7 @@
         <v>40</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>50</v>
@@ -3599,21 +3594,21 @@
         <v>40</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3636,16 +3631,16 @@
         <v>51</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>184</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>185</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>186</v>
       </c>
-      <c r="K20" t="s" s="2">
+      <c r="M20" t="s" s="2">
         <v>187</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>188</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>189</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
@@ -3695,7 +3690,7 @@
         <v>40</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>41</v>
@@ -3710,21 +3705,21 @@
         <v>40</v>
       </c>
       <c r="AJ20" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="AK20" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="AL20" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="AK20" t="s" s="2">
+      <c r="AM20" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="AL20" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="AM20" t="s" s="2">
-        <v>193</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3747,16 +3742,16 @@
         <v>51</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>195</v>
       </c>
-      <c r="K21" t="s" s="2">
+      <c r="M21" t="s" s="2">
         <v>196</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M21" t="s" s="2">
-        <v>198</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
@@ -3806,7 +3801,7 @@
         <v>40</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>41</v>
@@ -3821,21 +3816,21 @@
         <v>40</v>
       </c>
       <c r="AJ21" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="AK21" t="s" s="2">
+        <v>198</v>
+      </c>
+      <c r="AL21" t="s" s="2">
         <v>199</v>
       </c>
-      <c r="AK21" t="s" s="2">
+      <c r="AM21" t="s" s="2">
         <v>200</v>
-      </c>
-      <c r="AL21" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="AM21" t="s" s="2">
-        <v>202</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3858,16 +3853,16 @@
         <v>51</v>
       </c>
       <c r="J22" t="s" s="2">
+        <v>202</v>
+      </c>
+      <c r="K22" t="s" s="2">
+        <v>203</v>
+      </c>
+      <c r="L22" t="s" s="2">
         <v>204</v>
       </c>
-      <c r="K22" t="s" s="2">
+      <c r="M22" t="s" s="2">
         <v>205</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>207</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -3917,7 +3912,7 @@
         <v>40</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>41</v>
@@ -3932,7 +3927,7 @@
         <v>40</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>40</v>
@@ -3946,7 +3941,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3969,16 +3964,16 @@
         <v>51</v>
       </c>
       <c r="J23" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="L23" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="K23" t="s" s="2">
+      <c r="M23" t="s" s="2">
         <v>211</v>
-      </c>
-      <c r="L23" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>213</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
@@ -4028,7 +4023,7 @@
         <v>40</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>41</v>
@@ -4040,10 +4035,10 @@
         <v>40</v>
       </c>
       <c r="AI23" t="s" s="2">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>40</v>
@@ -4057,7 +4052,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4080,13 +4075,13 @@
         <v>40</v>
       </c>
       <c r="J24" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L24" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="K24" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="L24" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -4137,7 +4132,7 @@
         <v>40</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>41</v>
@@ -4152,7 +4147,7 @@
         <v>40</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>40</v>
@@ -4166,7 +4161,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4195,7 +4190,7 @@
         <v>97</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M25" t="s" s="2">
         <v>99</v>
@@ -4248,7 +4243,7 @@
         <v>40</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>41</v>
@@ -4263,7 +4258,7 @@
         <v>40</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>40</v>
@@ -4277,11 +4272,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4306,7 +4301,7 @@
         <v>102</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M26" t="s" s="2">
         <v>99</v>
@@ -4359,7 +4354,7 @@
         <v>40</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>41</v>
@@ -4388,7 +4383,7 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4414,13 +4409,13 @@
         <v>69</v>
       </c>
       <c r="K27" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="L27" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="M27" t="s" s="2">
         <v>230</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>232</v>
       </c>
       <c r="N27" s="2"/>
       <c r="O27" t="s" s="2">
@@ -4449,57 +4444,57 @@
         <v>125</v>
       </c>
       <c r="X27" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE27" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AF27" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AG27" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ27" t="s" s="2">
         <v>233</v>
       </c>
-      <c r="Y27" t="s" s="2">
+      <c r="AK27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL27" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM27" t="s" s="2">
         <v>234</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="AF27" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AG27" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ27" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="AK27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL27" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM27" t="s" s="2">
-        <v>236</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4522,13 +4517,13 @@
         <v>51</v>
       </c>
       <c r="J28" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="K28" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="L28" t="s" s="2">
         <v>238</v>
-      </c>
-      <c r="K28" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>240</v>
       </c>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -4579,7 +4574,7 @@
         <v>40</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>50</v>
@@ -4594,7 +4589,7 @@
         <v>40</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>40</v>
@@ -4603,12 +4598,12 @@
         <v>40</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4631,19 +4626,19 @@
         <v>51</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="M29" t="s" s="2">
         <v>244</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>245</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>247</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>40</v>
@@ -4692,7 +4687,7 @@
         <v>40</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>41</v>
@@ -4707,21 +4702,21 @@
         <v>40</v>
       </c>
       <c r="AJ29" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL29" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AM29" t="s" s="2">
         <v>248</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL29" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="AM29" t="s" s="2">
-        <v>250</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4747,16 +4742,16 @@
         <v>140</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>252</v>
       </c>
-      <c r="L30" t="s" s="2">
+      <c r="N30" t="s" s="2">
         <v>253</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>255</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>40</v>
@@ -4784,10 +4779,10 @@
         <v>73</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>40</v>
@@ -4805,7 +4800,7 @@
         <v>40</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>41</v>
@@ -4820,21 +4815,21 @@
         <v>40</v>
       </c>
       <c r="AJ30" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="AK30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL30" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="AM30" t="s" s="2">
         <v>258</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL30" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="AM30" t="s" s="2">
-        <v>260</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4857,13 +4852,13 @@
         <v>51</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M31" s="2"/>
       <c r="N31" s="2"/>
@@ -4914,7 +4909,7 @@
         <v>40</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>50</v>
@@ -4926,10 +4921,10 @@
         <v>40</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>40</v>
@@ -4943,7 +4938,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -4966,13 +4961,13 @@
         <v>40</v>
       </c>
       <c r="J32" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L32" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="K32" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2"/>
@@ -5023,7 +5018,7 @@
         <v>40</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>41</v>
@@ -5038,7 +5033,7 @@
         <v>40</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>40</v>
@@ -5052,7 +5047,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5081,7 +5076,7 @@
         <v>97</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M33" t="s" s="2">
         <v>99</v>
@@ -5134,7 +5129,7 @@
         <v>40</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>41</v>
@@ -5149,7 +5144,7 @@
         <v>40</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>40</v>
@@ -5163,11 +5158,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5192,7 +5187,7 @@
         <v>102</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>99</v>
@@ -5245,7 +5240,7 @@
         <v>40</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>41</v>
@@ -5274,7 +5269,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -5297,13 +5292,13 @@
         <v>51</v>
       </c>
       <c r="J35" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>269</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>271</v>
       </c>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
@@ -5354,7 +5349,7 @@
         <v>40</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>50</v>
@@ -5369,21 +5364,21 @@
         <v>40</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>40</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5406,13 +5401,13 @@
         <v>40</v>
       </c>
       <c r="J36" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K36" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L36" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="K36" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5463,7 +5458,7 @@
         <v>40</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>41</v>
@@ -5478,7 +5473,7 @@
         <v>40</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>40</v>
@@ -5492,7 +5487,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5521,7 +5516,7 @@
         <v>97</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>99</v>
@@ -5562,19 +5557,19 @@
         <v>40</v>
       </c>
       <c r="AA37" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD37" t="s" s="2">
         <v>276</v>
       </c>
-      <c r="AB37" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>278</v>
-      </c>
       <c r="AE37" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>41</v>
@@ -5589,7 +5584,7 @@
         <v>40</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>40</v>
@@ -5603,7 +5598,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5629,14 +5624,14 @@
         <v>69</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M38" s="2"/>
       <c r="N38" t="s" s="2">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>40</v>
@@ -5649,7 +5644,7 @@
         <v>40</v>
       </c>
       <c r="S38" t="s" s="2">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="T38" t="s" s="2">
         <v>40</v>
@@ -5664,49 +5659,49 @@
         <v>125</v>
       </c>
       <c r="X38" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="Y38" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="Z38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE38" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="Y38" t="s" s="2">
+      <c r="AF38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="Z38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE38" t="s" s="2">
+      <c r="AK38" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL38" t="s" s="2">
         <v>286</v>
-      </c>
-      <c r="AF38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>287</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL38" t="s" s="2">
-        <v>288</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>40</v>
@@ -5714,7 +5709,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5740,14 +5735,14 @@
         <v>69</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" t="s" s="2">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>40</v>
@@ -5760,7 +5755,7 @@
         <v>40</v>
       </c>
       <c r="S39" t="s" s="2">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="T39" t="s" s="2">
         <v>40</v>
@@ -5796,7 +5791,7 @@
         <v>40</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>41</v>
@@ -5811,7 +5806,7 @@
         <v>40</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>40</v>
@@ -5825,7 +5820,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -5848,19 +5843,19 @@
         <v>40</v>
       </c>
       <c r="J40" t="s" s="2">
+        <v>295</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>296</v>
+      </c>
+      <c r="L40" t="s" s="2">
         <v>297</v>
       </c>
-      <c r="K40" t="s" s="2">
+      <c r="M40" t="s" s="2">
         <v>298</v>
       </c>
-      <c r="L40" t="s" s="2">
+      <c r="N40" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="M40" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>40</v>
@@ -5909,28 +5904,28 @@
         <v>40</v>
       </c>
       <c r="AE40" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL40" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL40" t="s" s="2">
-        <v>304</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>40</v>
@@ -5938,7 +5933,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -5964,16 +5959,16 @@
         <v>63</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="M41" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="L41" t="s" s="2">
+      <c r="N41" t="s" s="2">
         <v>307</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>309</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>40</v>
@@ -5986,64 +5981,64 @@
         <v>40</v>
       </c>
       <c r="S41" t="s" s="2">
+        <v>308</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
         <v>310</v>
       </c>
-      <c r="T41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE41" t="s" s="2">
+      <c r="AK41" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL41" t="s" s="2">
         <v>311</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL41" t="s" s="2">
-        <v>313</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>40</v>
@@ -6051,7 +6046,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6074,19 +6069,19 @@
         <v>51</v>
       </c>
       <c r="J42" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="L42" t="s" s="2">
         <v>315</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="M42" t="s" s="2">
         <v>316</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="N42" t="s" s="2">
         <v>317</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>318</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>319</v>
       </c>
       <c r="O42" t="s" s="2">
         <v>40</v>
@@ -6135,7 +6130,7 @@
         <v>40</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>41</v>
@@ -6150,7 +6145,7 @@
         <v>40</v>
       </c>
       <c r="AJ42" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AK42" t="s" s="2">
         <v>40</v>
@@ -6164,7 +6159,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6187,19 +6182,19 @@
         <v>51</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="M43" t="s" s="2">
         <v>323</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>324</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="O43" t="s" s="2">
         <v>40</v>
@@ -6248,7 +6243,7 @@
         <v>40</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>41</v>
@@ -6263,7 +6258,7 @@
         <v>40</v>
       </c>
       <c r="AJ43" t="s" s="2">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AK43" t="s" s="2">
         <v>40</v>
@@ -6277,7 +6272,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6300,17 +6295,17 @@
         <v>51</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M44" s="2"/>
       <c r="N44" t="s" s="2">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>40</v>
@@ -6323,58 +6318,58 @@
         <v>40</v>
       </c>
       <c r="S44" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="U44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="V44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="W44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="X44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Y44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="Z44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE44" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="AF44" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG44" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI44" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ44" t="s" s="2">
         <v>333</v>
-      </c>
-      <c r="T44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="U44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="V44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="W44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="X44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Y44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE44" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="AF44" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG44" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI44" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ44" t="s" s="2">
-        <v>335</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>40</v>
@@ -6388,7 +6383,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6411,17 +6406,17 @@
         <v>51</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" t="s" s="2">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="O45" t="s" s="2">
         <v>40</v>
@@ -6470,7 +6465,7 @@
         <v>40</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>41</v>
@@ -6485,7 +6480,7 @@
         <v>40</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>40</v>
@@ -6499,7 +6494,7 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6522,16 +6517,16 @@
         <v>51</v>
       </c>
       <c r="J46" t="s" s="2">
+        <v>340</v>
+      </c>
+      <c r="K46" t="s" s="2">
+        <v>341</v>
+      </c>
+      <c r="L46" t="s" s="2">
         <v>342</v>
       </c>
-      <c r="K46" t="s" s="2">
+      <c r="M46" t="s" s="2">
         <v>343</v>
-      </c>
-      <c r="L46" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>345</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6561,7 +6556,7 @@
       </c>
       <c r="X46" s="2"/>
       <c r="Y46" t="s" s="2">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="Z46" t="s" s="2">
         <v>40</v>
@@ -6579,7 +6574,7 @@
         <v>40</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>41</v>
@@ -6594,7 +6589,7 @@
         <v>40</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>40</v>
@@ -6603,12 +6598,12 @@
         <v>40</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
@@ -6631,16 +6626,16 @@
         <v>51</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K47" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="L47" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="M47" t="s" s="2">
         <v>349</v>
-      </c>
-      <c r="L47" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="M47" t="s" s="2">
-        <v>351</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
@@ -6690,7 +6685,7 @@
         <v>40</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>41</v>
@@ -6702,10 +6697,10 @@
         <v>40</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>40</v>
@@ -6719,7 +6714,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -6742,13 +6737,13 @@
         <v>40</v>
       </c>
       <c r="J48" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K48" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L48" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="K48" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="L48" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M48" s="2"/>
       <c r="N48" s="2"/>
@@ -6799,7 +6794,7 @@
         <v>40</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>41</v>
@@ -6814,7 +6809,7 @@
         <v>40</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>40</v>
@@ -6828,7 +6823,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -6857,7 +6852,7 @@
         <v>97</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M49" t="s" s="2">
         <v>99</v>
@@ -6910,7 +6905,7 @@
         <v>40</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>41</v>
@@ -6925,7 +6920,7 @@
         <v>40</v>
       </c>
       <c r="AJ49" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK49" t="s" s="2">
         <v>40</v>
@@ -6939,11 +6934,11 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
@@ -6968,7 +6963,7 @@
         <v>102</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M50" t="s" s="2">
         <v>99</v>
@@ -7021,7 +7016,7 @@
         <v>40</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>41</v>
@@ -7050,7 +7045,7 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7073,13 +7068,13 @@
         <v>51</v>
       </c>
       <c r="J51" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="K51" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="L51" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="K51" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="L51" t="s" s="2">
-        <v>359</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -7130,7 +7125,7 @@
         <v>40</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>41</v>
@@ -7145,10 +7140,10 @@
         <v>40</v>
       </c>
       <c r="AJ51" t="s" s="2">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>40</v>
@@ -7159,7 +7154,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7185,13 +7180,13 @@
         <v>140</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>363</v>
-      </c>
-      <c r="L52" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>365</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" t="s" s="2">
@@ -7217,14 +7212,14 @@
         <v>40</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>156</v>
+        <v>364</v>
       </c>
       <c r="X52" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="Y52" t="s" s="2">
         <v>366</v>
       </c>
-      <c r="Y52" t="s" s="2">
-        <v>367</v>
-      </c>
       <c r="Z52" t="s" s="2">
         <v>40</v>
       </c>
@@ -7241,7 +7236,7 @@
         <v>40</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>41</v>
@@ -7256,21 +7251,21 @@
         <v>40</v>
       </c>
       <c r="AJ52" t="s" s="2">
+        <v>367</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>368</v>
-      </c>
-      <c r="AK52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL52" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM52" t="s" s="2">
-        <v>369</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7293,13 +7288,13 @@
         <v>51</v>
       </c>
       <c r="J53" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="K53" t="s" s="2">
         <v>371</v>
       </c>
-      <c r="K53" t="s" s="2">
+      <c r="L53" t="s" s="2">
         <v>372</v>
-      </c>
-      <c r="L53" t="s" s="2">
-        <v>373</v>
       </c>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
@@ -7350,7 +7345,7 @@
         <v>40</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>41</v>
@@ -7365,21 +7360,21 @@
         <v>40</v>
       </c>
       <c r="AJ53" t="s" s="2">
+        <v>373</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM53" t="s" s="2">
         <v>374</v>
-      </c>
-      <c r="AK53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL53" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM53" t="s" s="2">
-        <v>375</v>
       </c>
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" t="s" s="2">
@@ -7405,10 +7400,10 @@
         <v>140</v>
       </c>
       <c r="K54" t="s" s="2">
+        <v>376</v>
+      </c>
+      <c r="L54" t="s" s="2">
         <v>377</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>378</v>
       </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
@@ -7435,60 +7430,60 @@
         <v>40</v>
       </c>
       <c r="W54" t="s" s="2">
-        <v>156</v>
+        <v>364</v>
       </c>
       <c r="X54" t="s" s="2">
+        <v>378</v>
+      </c>
+      <c r="Y54" t="s" s="2">
         <v>379</v>
       </c>
-      <c r="Y54" t="s" s="2">
+      <c r="Z54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>375</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="Z54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>376</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
+      <c r="AK54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM54" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>382</v>
       </c>
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" t="s" s="2">
@@ -7514,16 +7509,16 @@
         <v>140</v>
       </c>
       <c r="K55" t="s" s="2">
+        <v>383</v>
+      </c>
+      <c r="L55" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="L55" t="s" s="2">
+      <c r="M55" t="s" s="2">
         <v>385</v>
       </c>
-      <c r="M55" t="s" s="2">
+      <c r="N55" t="s" s="2">
         <v>386</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>387</v>
       </c>
       <c r="O55" t="s" s="2">
         <v>40</v>
@@ -7548,60 +7543,60 @@
         <v>40</v>
       </c>
       <c r="W55" t="s" s="2">
-        <v>156</v>
+        <v>364</v>
       </c>
       <c r="X55" t="s" s="2">
+        <v>387</v>
+      </c>
+      <c r="Y55" t="s" s="2">
         <v>388</v>
       </c>
-      <c r="Y55" t="s" s="2">
+      <c r="Z55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>382</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM55" t="s" s="2">
         <v>389</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>381</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>390</v>
       </c>
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" t="s" s="2">
@@ -7624,13 +7619,13 @@
         <v>51</v>
       </c>
       <c r="J56" t="s" s="2">
+        <v>391</v>
+      </c>
+      <c r="K56" t="s" s="2">
         <v>392</v>
       </c>
-      <c r="K56" t="s" s="2">
+      <c r="L56" t="s" s="2">
         <v>393</v>
-      </c>
-      <c r="L56" t="s" s="2">
-        <v>394</v>
       </c>
       <c r="M56" s="2"/>
       <c r="N56" s="2"/>
@@ -7681,7 +7676,7 @@
         <v>40</v>
       </c>
       <c r="AE56" t="s" s="2">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="AF56" t="s" s="2">
         <v>41</v>
@@ -7696,7 +7691,7 @@
         <v>40</v>
       </c>
       <c r="AJ56" t="s" s="2">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AK56" t="s" s="2">
         <v>40</v>
@@ -7705,12 +7700,12 @@
         <v>40</v>
       </c>
       <c r="AM56" t="s" s="2">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" t="s" s="2">
@@ -7733,16 +7728,16 @@
         <v>51</v>
       </c>
       <c r="J57" t="s" s="2">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>396</v>
+      </c>
+      <c r="L57" t="s" s="2">
         <v>397</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="M57" t="s" s="2">
         <v>398</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>399</v>
       </c>
       <c r="N57" s="2"/>
       <c r="O57" t="s" s="2">
@@ -7792,7 +7787,7 @@
         <v>40</v>
       </c>
       <c r="AE57" t="s" s="2">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AF57" t="s" s="2">
         <v>41</v>
@@ -7804,24 +7799,24 @@
         <v>40</v>
       </c>
       <c r="AI57" t="s" s="2">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="AJ57" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="AK57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AL57" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AM57" t="s" s="2">
         <v>400</v>
-      </c>
-      <c r="AK57" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AL57" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AM57" t="s" s="2">
-        <v>401</v>
       </c>
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" t="s" s="2">
@@ -7844,13 +7839,13 @@
         <v>40</v>
       </c>
       <c r="J58" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="K58" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L58" t="s" s="2">
         <v>217</v>
-      </c>
-      <c r="K58" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="L58" t="s" s="2">
-        <v>219</v>
       </c>
       <c r="M58" s="2"/>
       <c r="N58" s="2"/>
@@ -7901,7 +7896,7 @@
         <v>40</v>
       </c>
       <c r="AE58" t="s" s="2">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="AF58" t="s" s="2">
         <v>41</v>
@@ -7916,7 +7911,7 @@
         <v>40</v>
       </c>
       <c r="AJ58" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK58" t="s" s="2">
         <v>40</v>
@@ -7930,7 +7925,7 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" t="s" s="2">
@@ -7959,7 +7954,7 @@
         <v>97</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M59" t="s" s="2">
         <v>99</v>
@@ -8012,7 +8007,7 @@
         <v>40</v>
       </c>
       <c r="AE59" t="s" s="2">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AF59" t="s" s="2">
         <v>41</v>
@@ -8027,7 +8022,7 @@
         <v>40</v>
       </c>
       <c r="AJ59" t="s" s="2">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="AK59" t="s" s="2">
         <v>40</v>
@@ -8041,11 +8036,11 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" t="s" s="2">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" t="s" s="2">
@@ -8070,7 +8065,7 @@
         <v>102</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M60" t="s" s="2">
         <v>99</v>
@@ -8123,7 +8118,7 @@
         <v>40</v>
       </c>
       <c r="AE60" t="s" s="2">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="AF60" t="s" s="2">
         <v>41</v>
@@ -8152,7 +8147,7 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" t="s" s="2">
@@ -8178,13 +8173,13 @@
         <v>106</v>
       </c>
       <c r="K61" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="L61" t="s" s="2">
         <v>406</v>
       </c>
-      <c r="L61" t="s" s="2">
+      <c r="M61" t="s" s="2">
         <v>407</v>
-      </c>
-      <c r="M61" t="s" s="2">
-        <v>408</v>
       </c>
       <c r="N61" s="2"/>
       <c r="O61" t="s" s="2">
@@ -8234,7 +8229,7 @@
         <v>40</v>
       </c>
       <c r="AE61" t="s" s="2">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="AF61" t="s" s="2">
         <v>41</v>
@@ -8249,7 +8244,7 @@
         <v>40</v>
       </c>
       <c r="AJ61" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AK61" t="s" s="2">
         <v>40</v>
@@ -8263,7 +8258,7 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" t="s" s="2">
@@ -8286,16 +8281,16 @@
         <v>51</v>
       </c>
       <c r="J62" t="s" s="2">
+        <v>410</v>
+      </c>
+      <c r="K62" t="s" s="2">
         <v>411</v>
       </c>
-      <c r="K62" t="s" s="2">
+      <c r="L62" t="s" s="2">
         <v>412</v>
       </c>
-      <c r="L62" t="s" s="2">
+      <c r="M62" t="s" s="2">
         <v>413</v>
-      </c>
-      <c r="M62" t="s" s="2">
-        <v>414</v>
       </c>
       <c r="N62" s="2"/>
       <c r="O62" t="s" s="2">
@@ -8345,7 +8340,7 @@
         <v>40</v>
       </c>
       <c r="AE62" t="s" s="2">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="AF62" t="s" s="2">
         <v>41</v>
@@ -8360,7 +8355,7 @@
         <v>40</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="AK62" t="s" s="2">
         <v>40</v>

</xml_diff>

<commit_message>
added DocumentReference.indexed requirement from STU#
</commit_message>
<xml_diff>
--- a/docs/cn-plus-uscore.xlsx
+++ b/docs/cn-plus-uscore.xlsx
@@ -3495,7 +3495,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
         <v>176</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>50</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>40</v>

</xml_diff>